<commit_message>
fix issue, service cannot be delete when it is running
</commit_message>
<xml_diff>
--- a/Misc/autolist2.0.xlsx
+++ b/Misc/autolist2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\HPEasyShell\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B31088C-9B45-4718-98AD-B342EB39AC96}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009BDE2-976C-4F72-A5EC-58EB4D9D0804}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="262">
   <si>
     <t>Feature</t>
   </si>
@@ -683,10 +683,6 @@
     <t>桌面池不稳定</t>
   </si>
   <si>
-    <t>1.桌面池不稳定
-2. Wifi列表是一张图片，不能通过选择添加，只能通过搜索按键添加</t>
-  </si>
-  <si>
     <t>Exit shutdown动作会影响测试</t>
   </si>
   <si>
@@ -721,9 +717,6 @@
     <t>电池只适应于NOTEPAD</t>
   </si>
   <si>
-    <t>电量无法控制</t>
-  </si>
-  <si>
     <t>外设性能无法检测</t>
   </si>
   <si>
@@ -829,7 +822,17 @@
     <t>settings_x21</t>
   </si>
   <si>
-    <t>Display detail information within email</t>
+    <t>1.桌面池不稳定
+2. Wifi列表是一张图片，不能通过选择添加，只能通过搜索按键添加, 与实际不一样</t>
+  </si>
+  <si>
+    <t>Display detail information within email when test finished</t>
+  </si>
+  <si>
+    <t>高低电量无法控制</t>
+  </si>
+  <si>
+    <t>wifi列表是一张图片，不能去选择；无法对外设键盘物理操作</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1155,6 +1158,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1451,8 +1460,8 @@
   <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1546,7 +1555,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>9</v>
@@ -1798,7 +1807,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" hidden="1">
       <c r="A16" s="24"/>
       <c r="B16" s="24" t="s">
         <v>36</v>
@@ -1903,7 +1912,7 @@
       <c r="H20" s="31"/>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" spans="1:9" ht="29.25" customHeight="1">
+    <row r="21" spans="1:9" ht="29.25" hidden="1" customHeight="1">
       <c r="A21" s="24" t="s">
         <v>42</v>
       </c>
@@ -1920,8 +1929,8 @@
       <c r="F21" s="24">
         <v>2</v>
       </c>
-      <c r="G21" s="33" t="s">
-        <v>213</v>
+      <c r="G21" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="H21" s="31"/>
       <c r="I21" s="29"/>
@@ -1942,12 +1951,12 @@
         <v>2</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H22" s="31"/>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" spans="1:9" ht="30">
+    <row r="23" spans="1:9" ht="45" hidden="1">
       <c r="A23" s="24"/>
       <c r="B23" s="24" t="s">
         <v>45</v>
@@ -1962,13 +1971,13 @@
       <c r="F23" s="24">
         <v>2</v>
       </c>
-      <c r="G23" s="33" t="s">
-        <v>213</v>
+      <c r="G23" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="H23" s="31"/>
       <c r="I23" s="29"/>
     </row>
-    <row r="24" spans="1:9" ht="30">
+    <row r="24" spans="1:9" ht="45" hidden="1">
       <c r="A24" s="24"/>
       <c r="B24" s="24" t="s">
         <v>46</v>
@@ -1983,13 +1992,13 @@
       <c r="F24" s="24">
         <v>2</v>
       </c>
-      <c r="G24" s="33" t="s">
-        <v>213</v>
+      <c r="G24" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="H24" s="31"/>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="1:9" ht="30">
+    <row r="25" spans="1:9" ht="45" hidden="1">
       <c r="A25" s="24"/>
       <c r="B25" s="24" t="s">
         <v>47</v>
@@ -2004,13 +2013,13 @@
       <c r="F25" s="24">
         <v>2</v>
       </c>
-      <c r="G25" s="33" t="s">
-        <v>213</v>
+      <c r="G25" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="H25" s="31"/>
       <c r="I25" s="29"/>
     </row>
-    <row r="26" spans="1:9" ht="30">
+    <row r="26" spans="1:9" ht="45" hidden="1">
       <c r="A26" s="24"/>
       <c r="B26" s="24" t="s">
         <v>48</v>
@@ -2025,13 +2034,13 @@
       <c r="F26" s="24">
         <v>2</v>
       </c>
-      <c r="G26" s="33" t="s">
-        <v>213</v>
+      <c r="G26" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="H26" s="31"/>
       <c r="I26" s="29"/>
     </row>
-    <row r="27" spans="1:9" ht="30">
+    <row r="27" spans="1:9" ht="45" hidden="1">
       <c r="A27" s="24"/>
       <c r="B27" s="24" t="s">
         <v>49</v>
@@ -2046,13 +2055,13 @@
       <c r="F27" s="24">
         <v>2</v>
       </c>
-      <c r="G27" s="33" t="s">
-        <v>213</v>
+      <c r="G27" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="H27" s="31"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="1:9" ht="30">
+    <row r="28" spans="1:9" ht="45" hidden="1">
       <c r="A28" s="24"/>
       <c r="B28" s="24" t="s">
         <v>50</v>
@@ -2067,8 +2076,8 @@
       <c r="F28" s="24">
         <v>2</v>
       </c>
-      <c r="G28" s="33" t="s">
-        <v>213</v>
+      <c r="G28" s="48" t="s">
+        <v>258</v>
       </c>
       <c r="H28" s="31"/>
       <c r="I28" s="29"/>
@@ -2089,7 +2098,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H29" s="31"/>
       <c r="I29" s="29"/>
@@ -2110,7 +2119,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H30" s="31"/>
       <c r="I30" s="29"/>
@@ -2159,13 +2168,13 @@
       <c r="H32" s="3"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" ht="14.25" customHeight="1">
+    <row r="33" spans="1:9" ht="14.25" hidden="1" customHeight="1">
       <c r="A33" s="42"/>
       <c r="B33" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>9</v>
@@ -2219,7 +2228,7 @@
         <v>2</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H35" s="31"/>
       <c r="I35" s="29"/>
@@ -2240,12 +2249,12 @@
         <v>2</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H36" s="31"/>
       <c r="I36" s="29"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" hidden="1">
       <c r="A37" s="24"/>
       <c r="B37" s="24" t="s">
         <v>63</v>
@@ -2331,7 +2340,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" hidden="1">
       <c r="A41" s="24"/>
       <c r="B41" s="24" t="s">
         <v>70</v>
@@ -2373,7 +2382,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" hidden="1">
       <c r="A43" s="24"/>
       <c r="B43" s="24" t="s">
         <v>73</v>
@@ -2394,7 +2403,7 @@
       <c r="H43" s="31"/>
       <c r="I43" s="29"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" hidden="1">
       <c r="A44" s="24"/>
       <c r="B44" s="24" t="s">
         <v>74</v>
@@ -2415,7 +2424,7 @@
       <c r="H44" s="31"/>
       <c r="I44" s="29"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" hidden="1">
       <c r="A45" s="24"/>
       <c r="B45" s="24" t="s">
         <v>75</v>
@@ -2457,7 +2466,7 @@
       <c r="H46" s="31"/>
       <c r="I46" s="29"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" hidden="1">
       <c r="A47" s="24"/>
       <c r="B47" s="24" t="s">
         <v>77</v>
@@ -2478,7 +2487,7 @@
       <c r="H47" s="31"/>
       <c r="I47" s="29"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" hidden="1">
       <c r="A48" s="24"/>
       <c r="B48" s="24" t="s">
         <v>78</v>
@@ -2515,7 +2524,7 @@
         <v>2</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H49" s="31"/>
       <c r="I49" s="29"/>
@@ -2536,7 +2545,7 @@
         <v>3</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H50" s="31"/>
       <c r="I50" s="29"/>
@@ -2557,12 +2566,12 @@
         <v>2</v>
       </c>
       <c r="G51" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H51" s="31"/>
       <c r="I51" s="29"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" hidden="1">
       <c r="A52" s="24"/>
       <c r="B52" s="24" t="s">
         <v>82</v>
@@ -2583,7 +2592,7 @@
       <c r="H52" s="31"/>
       <c r="I52" s="29"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" hidden="1">
       <c r="A53" s="24"/>
       <c r="B53" s="24" t="s">
         <v>83</v>
@@ -2625,7 +2634,7 @@
       <c r="H54" s="31"/>
       <c r="I54" s="29"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" hidden="1">
       <c r="A55" s="24"/>
       <c r="B55" s="24" t="s">
         <v>85</v>
@@ -2646,7 +2655,7 @@
       <c r="H55" s="31"/>
       <c r="I55" s="29"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" hidden="1">
       <c r="A56" s="24"/>
       <c r="B56" s="24" t="s">
         <v>86</v>
@@ -2667,7 +2676,7 @@
       <c r="H56" s="31"/>
       <c r="I56" s="29"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" hidden="1">
       <c r="A57" s="24"/>
       <c r="B57" s="24" t="s">
         <v>87</v>
@@ -2703,7 +2712,7 @@
       <c r="F58" s="5">
         <v>3</v>
       </c>
-      <c r="G58" s="35" t="s">
+      <c r="G58" s="49" t="s">
         <v>202</v>
       </c>
       <c r="H58" s="31"/>
@@ -2753,7 +2762,7 @@
       <c r="H60" s="3"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" hidden="1">
       <c r="A61" s="24"/>
       <c r="B61" s="24" t="s">
         <v>94</v>
@@ -2795,7 +2804,7 @@
       <c r="H62" s="3"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" hidden="1">
       <c r="A63" s="24"/>
       <c r="B63" s="24" t="s">
         <v>97</v>
@@ -2816,7 +2825,7 @@
       <c r="H63" s="31"/>
       <c r="I63" s="29"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" hidden="1">
       <c r="A64" s="24"/>
       <c r="B64" s="24" t="s">
         <v>98</v>
@@ -2878,7 +2887,7 @@
         <v>2</v>
       </c>
       <c r="G66" s="35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H66" s="31"/>
       <c r="I66" s="29"/>
@@ -2906,7 +2915,7 @@
       <c r="H67" s="31"/>
       <c r="I67" s="29"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" hidden="1">
       <c r="A68" s="24"/>
       <c r="B68" s="24" t="s">
         <v>102</v>
@@ -2927,7 +2936,7 @@
       <c r="H68" s="31"/>
       <c r="I68" s="29"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" hidden="1">
       <c r="A69" s="24"/>
       <c r="B69" s="24" t="s">
         <v>103</v>
@@ -2948,7 +2957,7 @@
       <c r="H69" s="31"/>
       <c r="I69" s="29"/>
     </row>
-    <row r="70" spans="1:9" ht="17.25" customHeight="1">
+    <row r="70" spans="1:9" ht="17.25" hidden="1" customHeight="1">
       <c r="A70" s="24" t="s">
         <v>104</v>
       </c>
@@ -2971,7 +2980,7 @@
       <c r="H70" s="31"/>
       <c r="I70" s="29"/>
     </row>
-    <row r="71" spans="1:9" ht="15.75" customHeight="1">
+    <row r="71" spans="1:9" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="24"/>
       <c r="B71" s="24" t="s">
         <v>106</v>
@@ -2992,7 +3001,7 @@
       <c r="H71" s="31"/>
       <c r="I71" s="29"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" hidden="1">
       <c r="A72" s="24"/>
       <c r="B72" s="24" t="s">
         <v>107</v>
@@ -3021,7 +3030,7 @@
         <v>109</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D73" s="43" t="s">
         <v>9</v>
@@ -3042,7 +3051,7 @@
         <v>110</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D74" s="43" t="s">
         <v>9</v>
@@ -3063,7 +3072,7 @@
         <v>111</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D75" s="43" t="s">
         <v>9</v>
@@ -3084,7 +3093,7 @@
         <v>112</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D76" s="42" t="s">
         <v>9</v>
@@ -3103,7 +3112,7 @@
       <c r="A77" s="44"/>
       <c r="B77" s="44"/>
       <c r="C77" s="44" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D77" s="44" t="s">
         <v>9</v>
@@ -3118,7 +3127,7 @@
       <c r="A78" s="44"/>
       <c r="B78" s="44"/>
       <c r="C78" s="44" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D78" s="44" t="s">
         <v>9</v>
@@ -3133,7 +3142,7 @@
       <c r="A79" s="44"/>
       <c r="B79" s="44"/>
       <c r="C79" s="44" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D79" s="44" t="s">
         <v>9</v>
@@ -3148,7 +3157,7 @@
       <c r="A80" s="44"/>
       <c r="B80" s="44"/>
       <c r="C80" s="44" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D80" s="44" t="s">
         <v>9</v>
@@ -3163,7 +3172,7 @@
       <c r="A81" s="44"/>
       <c r="B81" s="44"/>
       <c r="C81" s="44" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D81" s="44" t="s">
         <v>9</v>
@@ -3215,7 +3224,7 @@
         <v>2</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H83" s="31"/>
       <c r="I83" s="29"/>
@@ -3238,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="G84" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H84" s="31"/>
       <c r="I84" s="29"/>
@@ -3348,7 +3357,7 @@
       <c r="H89" s="31"/>
       <c r="I89" s="29"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" hidden="1">
       <c r="A90" s="24" t="s">
         <v>127</v>
       </c>
@@ -3392,7 +3401,7 @@
       <c r="H91" s="3"/>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" hidden="1">
       <c r="A92" s="24" t="s">
         <v>131</v>
       </c>
@@ -3410,7 +3419,7 @@
         <v>2</v>
       </c>
       <c r="G92" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H92" s="31"/>
       <c r="I92" s="29"/>
@@ -3430,8 +3439,8 @@
       <c r="F93" s="5">
         <v>2</v>
       </c>
-      <c r="G93" s="35" t="s">
-        <v>224</v>
+      <c r="G93" s="49" t="s">
+        <v>260</v>
       </c>
       <c r="H93" s="31"/>
       <c r="I93" s="29"/>
@@ -3444,7 +3453,7 @@
         <v>135</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D94" s="43" t="s">
         <v>9</v>
@@ -3465,7 +3474,7 @@
         <v>136</v>
       </c>
       <c r="C95" s="42" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D95" s="43" t="s">
         <v>9</v>
@@ -3486,7 +3495,7 @@
         <v>137</v>
       </c>
       <c r="C96" s="42" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D96" s="43" t="s">
         <v>9</v>
@@ -3517,7 +3526,7 @@
         <v>2</v>
       </c>
       <c r="G97" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H97" s="31"/>
       <c r="I97" s="29"/>
@@ -3530,7 +3539,7 @@
         <v>140</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D98" s="43" t="s">
         <v>9</v>
@@ -3551,7 +3560,7 @@
         <v>141</v>
       </c>
       <c r="C99" s="42" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D99" s="43" t="s">
         <v>9</v>
@@ -3572,7 +3581,7 @@
         <v>142</v>
       </c>
       <c r="C100" s="42" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D100" s="43" t="s">
         <v>9</v>
@@ -3602,8 +3611,8 @@
       <c r="F101" s="5">
         <v>2</v>
       </c>
-      <c r="G101" s="35" t="s">
-        <v>226</v>
+      <c r="G101" s="49" t="s">
+        <v>261</v>
       </c>
       <c r="H101" s="31"/>
       <c r="I101" s="29"/>
@@ -3624,7 +3633,7 @@
         <v>2</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H102" s="31"/>
       <c r="I102" s="29"/>
@@ -3635,7 +3644,7 @@
         <v>145</v>
       </c>
       <c r="C103" s="42" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D103" s="43" t="s">
         <v>9</v>
@@ -3650,7 +3659,7 @@
       <c r="H103" s="31"/>
       <c r="I103" s="29"/>
     </row>
-    <row r="104" spans="1:9" ht="15" customHeight="1">
+    <row r="104" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A104" s="24"/>
       <c r="B104" s="24" t="s">
         <v>146</v>
@@ -3666,7 +3675,7 @@
         <v>2</v>
       </c>
       <c r="G104" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H104" s="31"/>
       <c r="I104" s="29"/>
@@ -3687,7 +3696,7 @@
         <v>3</v>
       </c>
       <c r="G105" s="38" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H105" s="31"/>
       <c r="I105" s="29"/>
@@ -3698,7 +3707,7 @@
         <v>148</v>
       </c>
       <c r="C106" s="42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D106" s="43" t="s">
         <v>9</v>
@@ -3775,7 +3784,7 @@
         <v>2</v>
       </c>
       <c r="G109" s="35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H109" s="31"/>
       <c r="I109" s="29"/>
@@ -3796,7 +3805,7 @@
         <v>2</v>
       </c>
       <c r="G110" s="35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H110" s="31"/>
       <c r="I110" s="29"/>
@@ -3847,13 +3856,13 @@
     </row>
     <row r="113" spans="1:9" customFormat="1" hidden="1">
       <c r="A113" s="44" t="s">
+        <v>247</v>
+      </c>
+      <c r="B113" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="C113" s="44" t="s">
         <v>249</v>
-      </c>
-      <c r="B113" s="44" t="s">
-        <v>250</v>
-      </c>
-      <c r="C113" s="44" t="s">
-        <v>251</v>
       </c>
       <c r="D113" s="44" t="s">
         <v>9</v>
@@ -3861,7 +3870,7 @@
       <c r="E113" s="17"/>
       <c r="F113" s="44"/>
       <c r="G113" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="7"/>
@@ -3903,7 +3912,7 @@
       </c>
       <c r="F115" s="5"/>
       <c r="G115" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H115" s="31"/>
       <c r="I115" s="29"/>
@@ -3922,7 +3931,7 @@
       </c>
       <c r="F116" s="5"/>
       <c r="G116" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H116" s="31"/>
       <c r="I116" s="29"/>
@@ -3941,7 +3950,7 @@
       </c>
       <c r="F117" s="5"/>
       <c r="G117" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H117" s="31"/>
       <c r="I117" s="29"/>
@@ -3960,7 +3969,7 @@
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H118" s="31"/>
       <c r="I118" s="29"/>
@@ -3979,7 +3988,7 @@
       </c>
       <c r="F119" s="5"/>
       <c r="G119" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H119" s="31"/>
       <c r="I119" s="29"/>
@@ -3998,7 +4007,7 @@
       </c>
       <c r="F120" s="5"/>
       <c r="G120" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H120" s="31"/>
       <c r="I120" s="29"/>
@@ -4017,7 +4026,7 @@
       </c>
       <c r="F121" s="5"/>
       <c r="G121" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H121" s="31"/>
       <c r="I121" s="29"/>
@@ -4030,7 +4039,7 @@
         <v>161</v>
       </c>
       <c r="C122" s="42" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D122" s="43" t="s">
         <v>9</v>
@@ -4051,7 +4060,7 @@
         <v>162</v>
       </c>
       <c r="C123" s="42" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D123" s="43" t="s">
         <v>9</v>
@@ -4114,7 +4123,7 @@
         <v>165</v>
       </c>
       <c r="C126" s="42" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D126" s="43" t="s">
         <v>9</v>
@@ -4166,7 +4175,7 @@
         <v>1</v>
       </c>
       <c r="G128" s="35" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H128" s="31"/>
       <c r="I128" s="29"/>
@@ -4187,7 +4196,7 @@
         <v>1</v>
       </c>
       <c r="G129" s="35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H129" s="31"/>
       <c r="I129" s="29"/>
@@ -4274,7 +4283,7 @@
       <c r="H133" s="3"/>
       <c r="I133" s="7"/>
     </row>
-    <row r="134" spans="1:9" ht="15" customHeight="1">
+    <row r="134" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A134" s="24"/>
       <c r="B134" s="24" t="s">
         <v>172</v>
@@ -4311,7 +4320,7 @@
         <v>3</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H135" s="31"/>
       <c r="I135" s="29"/>
@@ -4343,7 +4352,7 @@
         <v>185</v>
       </c>
       <c r="C137" s="42" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D137" s="43" t="s">
         <v>9</v>
@@ -4376,7 +4385,7 @@
         <v>2</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="7"/>
@@ -4423,7 +4432,7 @@
       <c r="H140" s="31"/>
       <c r="I140" s="29"/>
     </row>
-    <row r="141" spans="1:9" ht="15" customHeight="1">
+    <row r="141" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A141" s="24"/>
       <c r="B141" s="24" t="s">
         <v>189</v>
@@ -4442,7 +4451,7 @@
       <c r="H141" s="31"/>
       <c r="I141" s="29"/>
     </row>
-    <row r="142" spans="1:9" ht="15" customHeight="1">
+    <row r="142" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A142" s="24"/>
       <c r="B142" s="24" t="s">
         <v>190</v>
@@ -4471,7 +4480,6 @@
     <filterColumn colId="3">
       <filters>
         <filter val="N/A"/>
-        <filter val="Planning"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
update test plan template for hpeasyshell
</commit_message>
<xml_diff>
--- a/Misc/autolist2.0.xlsx
+++ b/Misc/autolist2.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\HPEasyShell\Misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\Funtion_HPEasyshell_test\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009BDE2-976C-4F72-A5EC-58EB4D9D0804}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2A05E3-4C13-4937-8764-63D86ABAA47B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="261">
   <si>
     <t>Feature</t>
   </si>
@@ -683,6 +683,10 @@
     <t>桌面池不稳定</t>
   </si>
   <si>
+    <t>1.桌面池不稳定
+2. Wifi列表是一张图片，不能通过选择添加，只能通过搜索按键添加</t>
+  </si>
+  <si>
     <t>Exit shutdown动作会影响测试</t>
   </si>
   <si>
@@ -717,6 +721,9 @@
     <t>电池只适应于NOTEPAD</t>
   </si>
   <si>
+    <t>电量无法控制</t>
+  </si>
+  <si>
     <t>外设性能无法检测</t>
   </si>
   <si>
@@ -822,17 +829,7 @@
     <t>settings_x21</t>
   </si>
   <si>
-    <t>1.桌面池不稳定
-2. Wifi列表是一张图片，不能通过选择添加，只能通过搜索按键添加, 与实际不一样</t>
-  </si>
-  <si>
-    <t>Display detail information within email when test finished</t>
-  </si>
-  <si>
-    <t>高低电量无法控制</t>
-  </si>
-  <si>
-    <t>wifi列表是一张图片，不能去选择；无法对外设键盘物理操作</t>
+    <t>Display detail information within email</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1016,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1151,20 +1148,14 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1460,8 +1451,8 @@
   <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1503,7 +1494,7 @@
       </c>
       <c r="I1" s="29"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="27" hidden="1" customHeight="1">
+    <row r="2" spans="1:9" customFormat="1" ht="27" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>6</v>
       </c>
@@ -1526,7 +1517,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" customFormat="1" hidden="1">
+    <row r="3" spans="1:9" customFormat="1">
       <c r="A3" s="42"/>
       <c r="B3" s="42" t="s">
         <v>11</v>
@@ -1549,13 +1540,13 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" hidden="1">
+    <row r="4" spans="1:9">
       <c r="A4" s="42"/>
       <c r="B4" s="42" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>9</v>
@@ -1570,7 +1561,7 @@
       <c r="H4" s="31"/>
       <c r="I4" s="29"/>
     </row>
-    <row r="5" spans="1:9" customFormat="1" hidden="1">
+    <row r="5" spans="1:9" customFormat="1">
       <c r="A5" s="42"/>
       <c r="B5" s="42" t="s">
         <v>14</v>
@@ -1593,7 +1584,7 @@
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" customFormat="1" hidden="1">
+    <row r="6" spans="1:9" customFormat="1">
       <c r="A6" s="42"/>
       <c r="B6" s="42" t="s">
         <v>16</v>
@@ -1614,7 +1605,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" customFormat="1" hidden="1">
+    <row r="7" spans="1:9" customFormat="1">
       <c r="A7" s="42"/>
       <c r="B7" s="42" t="s">
         <v>18</v>
@@ -1637,7 +1628,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" customFormat="1" hidden="1">
+    <row r="8" spans="1:9" customFormat="1">
       <c r="A8" s="42"/>
       <c r="B8" s="42" t="s">
         <v>20</v>
@@ -1658,7 +1649,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" customFormat="1" hidden="1">
+    <row r="9" spans="1:9" customFormat="1">
       <c r="A9" s="42"/>
       <c r="B9" s="42" t="s">
         <v>22</v>
@@ -1679,7 +1670,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" customFormat="1" hidden="1">
+    <row r="10" spans="1:9" customFormat="1">
       <c r="A10" s="42"/>
       <c r="B10" s="42" t="s">
         <v>24</v>
@@ -1700,7 +1691,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" hidden="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>26</v>
@@ -1721,7 +1712,7 @@
       <c r="H11" s="31"/>
       <c r="I11" s="29"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" hidden="1">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>28</v>
@@ -1742,7 +1733,7 @@
       <c r="H12" s="31"/>
       <c r="I12" s="29"/>
     </row>
-    <row r="13" spans="1:9" customFormat="1" ht="30" hidden="1">
+    <row r="13" spans="1:9" customFormat="1" ht="30">
       <c r="A13" s="42"/>
       <c r="B13" s="42" t="s">
         <v>29</v>
@@ -1763,7 +1754,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" customFormat="1" ht="33" hidden="1" customHeight="1">
+    <row r="14" spans="1:9" customFormat="1" ht="33" customHeight="1">
       <c r="A14" s="42" t="s">
         <v>31</v>
       </c>
@@ -1786,7 +1777,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" customFormat="1" hidden="1">
+    <row r="15" spans="1:9" customFormat="1">
       <c r="A15" s="42"/>
       <c r="B15" s="42" t="s">
         <v>34</v>
@@ -1828,7 +1819,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="1:9" customFormat="1" hidden="1">
+    <row r="17" spans="1:9" customFormat="1">
       <c r="A17" s="42"/>
       <c r="B17" s="42" t="s">
         <v>37</v>
@@ -1849,7 +1840,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" ht="30">
+    <row r="18" spans="1:9" ht="30" hidden="1">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>39</v>
@@ -1870,7 +1861,7 @@
       <c r="H18" s="31"/>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" spans="1:9" ht="30">
+    <row r="19" spans="1:9" ht="30" hidden="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6" t="s">
         <v>40</v>
@@ -1891,7 +1882,7 @@
       <c r="H19" s="31"/>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" hidden="1">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>41</v>
@@ -1929,13 +1920,13 @@
       <c r="F21" s="24">
         <v>2</v>
       </c>
-      <c r="G21" s="48" t="s">
-        <v>258</v>
+      <c r="G21" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="H21" s="31"/>
       <c r="I21" s="29"/>
     </row>
-    <row r="22" spans="1:9" ht="30">
+    <row r="22" spans="1:9" ht="30" hidden="1">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>44</v>
@@ -1951,12 +1942,12 @@
         <v>2</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H22" s="31"/>
       <c r="I22" s="29"/>
     </row>
-    <row r="23" spans="1:9" ht="45" hidden="1">
+    <row r="23" spans="1:9" ht="30" hidden="1">
       <c r="A23" s="24"/>
       <c r="B23" s="24" t="s">
         <v>45</v>
@@ -1971,13 +1962,13 @@
       <c r="F23" s="24">
         <v>2</v>
       </c>
-      <c r="G23" s="48" t="s">
-        <v>258</v>
+      <c r="G23" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="H23" s="31"/>
       <c r="I23" s="29"/>
     </row>
-    <row r="24" spans="1:9" ht="45" hidden="1">
+    <row r="24" spans="1:9" ht="30" hidden="1">
       <c r="A24" s="24"/>
       <c r="B24" s="24" t="s">
         <v>46</v>
@@ -1992,13 +1983,13 @@
       <c r="F24" s="24">
         <v>2</v>
       </c>
-      <c r="G24" s="48" t="s">
-        <v>258</v>
+      <c r="G24" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="H24" s="31"/>
       <c r="I24" s="29"/>
     </row>
-    <row r="25" spans="1:9" ht="45" hidden="1">
+    <row r="25" spans="1:9" ht="30" hidden="1">
       <c r="A25" s="24"/>
       <c r="B25" s="24" t="s">
         <v>47</v>
@@ -2013,13 +2004,13 @@
       <c r="F25" s="24">
         <v>2</v>
       </c>
-      <c r="G25" s="48" t="s">
-        <v>258</v>
+      <c r="G25" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="H25" s="31"/>
       <c r="I25" s="29"/>
     </row>
-    <row r="26" spans="1:9" ht="45" hidden="1">
+    <row r="26" spans="1:9" ht="30" hidden="1">
       <c r="A26" s="24"/>
       <c r="B26" s="24" t="s">
         <v>48</v>
@@ -2034,13 +2025,13 @@
       <c r="F26" s="24">
         <v>2</v>
       </c>
-      <c r="G26" s="48" t="s">
-        <v>258</v>
+      <c r="G26" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="H26" s="31"/>
       <c r="I26" s="29"/>
     </row>
-    <row r="27" spans="1:9" ht="45" hidden="1">
+    <row r="27" spans="1:9" ht="30" hidden="1">
       <c r="A27" s="24"/>
       <c r="B27" s="24" t="s">
         <v>49</v>
@@ -2055,13 +2046,13 @@
       <c r="F27" s="24">
         <v>2</v>
       </c>
-      <c r="G27" s="48" t="s">
-        <v>258</v>
+      <c r="G27" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="H27" s="31"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="1:9" ht="45" hidden="1">
+    <row r="28" spans="1:9" ht="30" hidden="1">
       <c r="A28" s="24"/>
       <c r="B28" s="24" t="s">
         <v>50</v>
@@ -2076,13 +2067,13 @@
       <c r="F28" s="24">
         <v>2</v>
       </c>
-      <c r="G28" s="48" t="s">
-        <v>258</v>
+      <c r="G28" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="H28" s="31"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" spans="1:9" ht="30">
+    <row r="29" spans="1:9" ht="30" hidden="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>51</v>
@@ -2098,12 +2089,12 @@
         <v>2</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H29" s="31"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" spans="1:9" ht="30">
+    <row r="30" spans="1:9" ht="30" hidden="1">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>52</v>
@@ -2119,12 +2110,12 @@
         <v>2</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H30" s="31"/>
       <c r="I30" s="29"/>
     </row>
-    <row r="31" spans="1:9" customFormat="1" ht="29.25" hidden="1" customHeight="1">
+    <row r="31" spans="1:9" customFormat="1" ht="29.25" customHeight="1">
       <c r="A31" s="42" t="s">
         <v>53</v>
       </c>
@@ -2147,7 +2138,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" customFormat="1" hidden="1">
+    <row r="32" spans="1:9" customFormat="1">
       <c r="A32" s="42"/>
       <c r="B32" s="42" t="s">
         <v>56</v>
@@ -2168,13 +2159,13 @@
       <c r="H32" s="3"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" ht="14.25" hidden="1" customHeight="1">
+    <row r="33" spans="1:9" ht="14.25" customHeight="1">
       <c r="A33" s="42"/>
       <c r="B33" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>9</v>
@@ -2191,7 +2182,7 @@
       <c r="H33" s="31"/>
       <c r="I33" s="29"/>
     </row>
-    <row r="34" spans="1:9" customFormat="1" ht="16.5" hidden="1" customHeight="1">
+    <row r="34" spans="1:9" customFormat="1" ht="16.5" customHeight="1">
       <c r="A34" s="42"/>
       <c r="B34" s="42" t="s">
         <v>59</v>
@@ -2212,7 +2203,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" hidden="1">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>61</v>
@@ -2228,12 +2219,12 @@
         <v>2</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H35" s="31"/>
       <c r="I35" s="29"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="30" hidden="1">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
         <v>62</v>
@@ -2249,12 +2240,12 @@
         <v>2</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H36" s="31"/>
       <c r="I36" s="29"/>
     </row>
-    <row r="37" spans="1:9" hidden="1">
+    <row r="37" spans="1:9" ht="30" hidden="1">
       <c r="A37" s="24"/>
       <c r="B37" s="24" t="s">
         <v>63</v>
@@ -2275,7 +2266,7 @@
       <c r="H37" s="31"/>
       <c r="I37" s="29"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" hidden="1">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
         <v>64</v>
@@ -2296,7 +2287,7 @@
       <c r="H38" s="31"/>
       <c r="I38" s="29"/>
     </row>
-    <row r="39" spans="1:9" customFormat="1" ht="21.75" hidden="1" customHeight="1">
+    <row r="39" spans="1:9" customFormat="1" ht="21.75" customHeight="1">
       <c r="A39" s="42" t="s">
         <v>65</v>
       </c>
@@ -2319,7 +2310,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" customFormat="1" hidden="1">
+    <row r="40" spans="1:9" customFormat="1">
       <c r="A40" s="42"/>
       <c r="B40" s="42" t="s">
         <v>68</v>
@@ -2361,7 +2352,7 @@
       <c r="H41" s="31"/>
       <c r="I41" s="29"/>
     </row>
-    <row r="42" spans="1:9" customFormat="1" hidden="1">
+    <row r="42" spans="1:9" customFormat="1">
       <c r="A42" s="42"/>
       <c r="B42" s="42" t="s">
         <v>71</v>
@@ -2445,7 +2436,7 @@
       <c r="H45" s="31"/>
       <c r="I45" s="29"/>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9" ht="30" hidden="1">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
         <v>76</v>
@@ -2487,7 +2478,7 @@
       <c r="H47" s="31"/>
       <c r="I47" s="29"/>
     </row>
-    <row r="48" spans="1:9" hidden="1">
+    <row r="48" spans="1:9" ht="30" hidden="1">
       <c r="A48" s="24"/>
       <c r="B48" s="24" t="s">
         <v>78</v>
@@ -2508,7 +2499,7 @@
       <c r="H48" s="31"/>
       <c r="I48" s="29"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" hidden="1">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
         <v>79</v>
@@ -2524,12 +2515,12 @@
         <v>2</v>
       </c>
       <c r="G49" s="34" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H49" s="31"/>
       <c r="I49" s="29"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" hidden="1">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
         <v>80</v>
@@ -2545,12 +2536,12 @@
         <v>3</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H50" s="31"/>
       <c r="I50" s="29"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" hidden="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
         <v>81</v>
@@ -2566,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="G51" s="35" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H51" s="31"/>
       <c r="I51" s="29"/>
@@ -2613,7 +2604,7 @@
       <c r="H53" s="31"/>
       <c r="I53" s="29"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" hidden="1">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
         <v>84</v>
@@ -2634,7 +2625,7 @@
       <c r="H54" s="31"/>
       <c r="I54" s="29"/>
     </row>
-    <row r="55" spans="1:9" hidden="1">
+    <row r="55" spans="1:9" ht="30" hidden="1">
       <c r="A55" s="24"/>
       <c r="B55" s="24" t="s">
         <v>85</v>
@@ -2697,7 +2688,7 @@
       <c r="H57" s="31"/>
       <c r="I57" s="29"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" hidden="1">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>88</v>
@@ -2712,13 +2703,13 @@
       <c r="F58" s="5">
         <v>3</v>
       </c>
-      <c r="G58" s="49" t="s">
+      <c r="G58" s="35" t="s">
         <v>202</v>
       </c>
       <c r="H58" s="31"/>
       <c r="I58" s="29"/>
     </row>
-    <row r="59" spans="1:9" customFormat="1" ht="25.5" hidden="1" customHeight="1">
+    <row r="59" spans="1:9" customFormat="1" ht="25.5" customHeight="1">
       <c r="A59" s="42" t="s">
         <v>89</v>
       </c>
@@ -2741,7 +2732,7 @@
       <c r="H59" s="3"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" customFormat="1" hidden="1">
+    <row r="60" spans="1:9" customFormat="1">
       <c r="A60" s="42"/>
       <c r="B60" s="42" t="s">
         <v>92</v>
@@ -2783,7 +2774,7 @@
       <c r="H61" s="31"/>
       <c r="I61" s="29"/>
     </row>
-    <row r="62" spans="1:9" customFormat="1" hidden="1">
+    <row r="62" spans="1:9" customFormat="1">
       <c r="A62" s="42"/>
       <c r="B62" s="42" t="s">
         <v>95</v>
@@ -2846,7 +2837,7 @@
       <c r="H64" s="31"/>
       <c r="I64" s="29"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" hidden="1">
       <c r="A65" s="4"/>
       <c r="B65" s="4" t="s">
         <v>99</v>
@@ -2869,7 +2860,7 @@
       <c r="H65" s="31"/>
       <c r="I65" s="29"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" ht="30" hidden="1">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
         <v>100</v>
@@ -2887,12 +2878,12 @@
         <v>2</v>
       </c>
       <c r="G66" s="35" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H66" s="31"/>
       <c r="I66" s="29"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" hidden="1">
       <c r="A67" s="4"/>
       <c r="B67" s="4" t="s">
         <v>101</v>
@@ -3022,7 +3013,7 @@
       <c r="H72" s="31"/>
       <c r="I72" s="29"/>
     </row>
-    <row r="73" spans="1:9" customFormat="1" ht="21.75" hidden="1" customHeight="1">
+    <row r="73" spans="1:9" customFormat="1" ht="21.75" customHeight="1">
       <c r="A73" s="42" t="s">
         <v>108</v>
       </c>
@@ -3030,7 +3021,7 @@
         <v>109</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D73" s="43" t="s">
         <v>9</v>
@@ -3045,13 +3036,13 @@
       <c r="H73" s="3"/>
       <c r="I73" s="7"/>
     </row>
-    <row r="74" spans="1:9" customFormat="1" hidden="1">
+    <row r="74" spans="1:9" customFormat="1">
       <c r="A74" s="42"/>
       <c r="B74" s="42" t="s">
         <v>110</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D74" s="43" t="s">
         <v>9</v>
@@ -3066,13 +3057,13 @@
       <c r="H74" s="3"/>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="1:9" customFormat="1" hidden="1">
+    <row r="75" spans="1:9" customFormat="1">
       <c r="A75" s="42"/>
       <c r="B75" s="42" t="s">
         <v>111</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D75" s="43" t="s">
         <v>9</v>
@@ -3087,13 +3078,13 @@
       <c r="H75" s="3"/>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="1:9" hidden="1">
+    <row r="76" spans="1:9">
       <c r="A76" s="42"/>
       <c r="B76" s="42" t="s">
         <v>112</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D76" s="42" t="s">
         <v>9</v>
@@ -3108,82 +3099,82 @@
       <c r="H76" s="31"/>
       <c r="I76" s="29"/>
     </row>
-    <row r="77" spans="1:9" hidden="1">
+    <row r="77" spans="1:9">
       <c r="A77" s="44"/>
       <c r="B77" s="44"/>
       <c r="C77" s="44" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D77" s="44" t="s">
         <v>9</v>
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="44"/>
-      <c r="G77" s="45"/>
+      <c r="G77" s="46"/>
       <c r="H77" s="31"/>
       <c r="I77" s="29"/>
     </row>
-    <row r="78" spans="1:9" hidden="1">
+    <row r="78" spans="1:9">
       <c r="A78" s="44"/>
       <c r="B78" s="44"/>
       <c r="C78" s="44" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D78" s="44" t="s">
         <v>9</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="44"/>
-      <c r="G78" s="45"/>
+      <c r="G78" s="46"/>
       <c r="H78" s="31"/>
       <c r="I78" s="29"/>
     </row>
-    <row r="79" spans="1:9" hidden="1">
+    <row r="79" spans="1:9">
       <c r="A79" s="44"/>
       <c r="B79" s="44"/>
       <c r="C79" s="44" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D79" s="44" t="s">
         <v>9</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="44"/>
-      <c r="G79" s="45"/>
+      <c r="G79" s="46"/>
       <c r="H79" s="31"/>
       <c r="I79" s="29"/>
     </row>
-    <row r="80" spans="1:9" hidden="1">
+    <row r="80" spans="1:9">
       <c r="A80" s="44"/>
       <c r="B80" s="44"/>
       <c r="C80" s="44" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D80" s="44" t="s">
         <v>9</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="44"/>
-      <c r="G80" s="45"/>
+      <c r="G80" s="46"/>
       <c r="H80" s="31"/>
       <c r="I80" s="29"/>
     </row>
-    <row r="81" spans="1:9" hidden="1">
+    <row r="81" spans="1:9">
       <c r="A81" s="44"/>
       <c r="B81" s="44"/>
       <c r="C81" s="44" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D81" s="44" t="s">
         <v>9</v>
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="44"/>
-      <c r="G81" s="46"/>
+      <c r="G81" s="47"/>
       <c r="H81" s="31"/>
       <c r="I81" s="29"/>
     </row>
-    <row r="82" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="82" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A82" s="42" t="s">
         <v>113</v>
       </c>
@@ -3206,7 +3197,7 @@
       <c r="H82" s="3"/>
       <c r="I82" s="7"/>
     </row>
-    <row r="83" spans="1:9" ht="15" customHeight="1">
+    <row r="83" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
         <v>116</v>
@@ -3224,12 +3215,12 @@
         <v>2</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H83" s="31"/>
       <c r="I83" s="29"/>
     </row>
-    <row r="84" spans="1:9" ht="15" customHeight="1">
+    <row r="84" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
         <v>117</v>
@@ -3247,12 +3238,12 @@
         <v>3</v>
       </c>
       <c r="G84" s="35" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H84" s="31"/>
       <c r="I84" s="29"/>
     </row>
-    <row r="85" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="85" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A85" s="42"/>
       <c r="B85" s="42" t="s">
         <v>118</v>
@@ -3273,7 +3264,7 @@
       <c r="H85" s="3"/>
       <c r="I85" s="7"/>
     </row>
-    <row r="86" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="86" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A86" s="42"/>
       <c r="B86" s="42" t="s">
         <v>120</v>
@@ -3294,7 +3285,7 @@
       <c r="H86" s="3"/>
       <c r="I86" s="7"/>
     </row>
-    <row r="87" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="87" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A87" s="42"/>
       <c r="B87" s="42" t="s">
         <v>122</v>
@@ -3315,7 +3306,7 @@
       <c r="H87" s="3"/>
       <c r="I87" s="7"/>
     </row>
-    <row r="88" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="88" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A88" s="42"/>
       <c r="B88" s="42" t="s">
         <v>124</v>
@@ -3336,7 +3327,7 @@
       <c r="H88" s="3"/>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="1:9" ht="15" customHeight="1">
+    <row r="89" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="4" t="s">
         <v>126</v>
@@ -3380,7 +3371,7 @@
       <c r="H90" s="31"/>
       <c r="I90" s="29"/>
     </row>
-    <row r="91" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="91" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A91" s="42"/>
       <c r="B91" s="42" t="s">
         <v>129</v>
@@ -3419,12 +3410,12 @@
         <v>2</v>
       </c>
       <c r="G92" s="33" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H92" s="31"/>
       <c r="I92" s="29"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" hidden="1">
       <c r="A93" s="4"/>
       <c r="B93" s="4" t="s">
         <v>133</v>
@@ -3439,13 +3430,13 @@
       <c r="F93" s="5">
         <v>2</v>
       </c>
-      <c r="G93" s="49" t="s">
-        <v>260</v>
+      <c r="G93" s="35" t="s">
+        <v>224</v>
       </c>
       <c r="H93" s="31"/>
       <c r="I93" s="29"/>
     </row>
-    <row r="94" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="94" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A94" s="42" t="s">
         <v>134</v>
       </c>
@@ -3453,7 +3444,7 @@
         <v>135</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D94" s="43" t="s">
         <v>9</v>
@@ -3468,13 +3459,13 @@
       <c r="H94" s="3"/>
       <c r="I94" s="7"/>
     </row>
-    <row r="95" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="95" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A95" s="42"/>
       <c r="B95" s="42" t="s">
         <v>136</v>
       </c>
       <c r="C95" s="42" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D95" s="43" t="s">
         <v>9</v>
@@ -3489,13 +3480,13 @@
       <c r="H95" s="3"/>
       <c r="I95" s="7"/>
     </row>
-    <row r="96" spans="1:9" customFormat="1" hidden="1">
+    <row r="96" spans="1:9" customFormat="1">
       <c r="A96" s="42"/>
       <c r="B96" s="42" t="s">
         <v>137</v>
       </c>
       <c r="C96" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D96" s="43" t="s">
         <v>9</v>
@@ -3510,7 +3501,7 @@
       <c r="H96" s="3"/>
       <c r="I96" s="7"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" hidden="1">
       <c r="A97" s="4"/>
       <c r="B97" s="4" t="s">
         <v>138</v>
@@ -3526,12 +3517,12 @@
         <v>2</v>
       </c>
       <c r="G97" s="35" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H97" s="31"/>
       <c r="I97" s="29"/>
     </row>
-    <row r="98" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="98" spans="1:9" ht="15" customHeight="1">
       <c r="A98" s="42" t="s">
         <v>139</v>
       </c>
@@ -3539,7 +3530,7 @@
         <v>140</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D98" s="43" t="s">
         <v>9</v>
@@ -3554,13 +3545,13 @@
       <c r="H98" s="31"/>
       <c r="I98" s="29"/>
     </row>
-    <row r="99" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="99" spans="1:9" ht="15" customHeight="1">
       <c r="A99" s="42"/>
       <c r="B99" s="42" t="s">
         <v>141</v>
       </c>
       <c r="C99" s="42" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D99" s="43" t="s">
         <v>9</v>
@@ -3575,13 +3566,13 @@
       <c r="H99" s="31"/>
       <c r="I99" s="29"/>
     </row>
-    <row r="100" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="100" spans="1:9" ht="15" customHeight="1">
       <c r="A100" s="42"/>
       <c r="B100" s="42" t="s">
         <v>142</v>
       </c>
       <c r="C100" s="42" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D100" s="43" t="s">
         <v>9</v>
@@ -3596,7 +3587,7 @@
       <c r="H100" s="31"/>
       <c r="I100" s="29"/>
     </row>
-    <row r="101" spans="1:9" ht="15" customHeight="1">
+    <row r="101" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="s">
         <v>143</v>
@@ -3611,13 +3602,13 @@
       <c r="F101" s="5">
         <v>2</v>
       </c>
-      <c r="G101" s="49" t="s">
-        <v>261</v>
+      <c r="G101" s="35" t="s">
+        <v>226</v>
       </c>
       <c r="H101" s="31"/>
       <c r="I101" s="29"/>
     </row>
-    <row r="102" spans="1:9" ht="15" customHeight="1">
+    <row r="102" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A102" s="5"/>
       <c r="B102" s="5" t="s">
         <v>144</v>
@@ -3633,18 +3624,18 @@
         <v>2</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H102" s="31"/>
       <c r="I102" s="29"/>
     </row>
-    <row r="103" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="103" spans="1:9" ht="15" customHeight="1">
       <c r="A103" s="42"/>
       <c r="B103" s="42" t="s">
         <v>145</v>
       </c>
       <c r="C103" s="42" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D103" s="43" t="s">
         <v>9</v>
@@ -3675,12 +3666,12 @@
         <v>2</v>
       </c>
       <c r="G104" s="33" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H104" s="31"/>
       <c r="I104" s="29"/>
     </row>
-    <row r="105" spans="1:9" ht="15" customHeight="1">
+    <row r="105" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A105" s="4"/>
       <c r="B105" s="4" t="s">
         <v>147</v>
@@ -3696,18 +3687,18 @@
         <v>3</v>
       </c>
       <c r="G105" s="38" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H105" s="31"/>
       <c r="I105" s="29"/>
     </row>
-    <row r="106" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="106" spans="1:9" ht="15" customHeight="1">
       <c r="A106" s="42"/>
       <c r="B106" s="42" t="s">
         <v>148</v>
       </c>
       <c r="C106" s="42" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D106" s="43" t="s">
         <v>9</v>
@@ -3722,7 +3713,7 @@
       <c r="H106" s="31"/>
       <c r="I106" s="29"/>
     </row>
-    <row r="107" spans="1:9" ht="15" customHeight="1">
+    <row r="107" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
         <v>149</v>
@@ -3743,7 +3734,7 @@
       <c r="H107" s="31"/>
       <c r="I107" s="29"/>
     </row>
-    <row r="108" spans="1:9" ht="15" customHeight="1">
+    <row r="108" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A108" s="4" t="s">
         <v>150</v>
       </c>
@@ -3766,7 +3757,7 @@
       <c r="H108" s="31"/>
       <c r="I108" s="29"/>
     </row>
-    <row r="109" spans="1:9" ht="15" customHeight="1">
+    <row r="109" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A109" s="4" t="s">
         <v>152</v>
       </c>
@@ -3784,12 +3775,12 @@
         <v>2</v>
       </c>
       <c r="G109" s="35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H109" s="31"/>
       <c r="I109" s="29"/>
     </row>
-    <row r="110" spans="1:9" ht="15" customHeight="1">
+    <row r="110" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
         <v>154</v>
@@ -3805,12 +3796,12 @@
         <v>2</v>
       </c>
       <c r="G110" s="35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H110" s="31"/>
       <c r="I110" s="29"/>
     </row>
-    <row r="111" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="111" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A111" s="42" t="s">
         <v>155</v>
       </c>
@@ -3833,7 +3824,7 @@
       <c r="H111" s="3"/>
       <c r="I111" s="7"/>
     </row>
-    <row r="112" spans="1:9" customFormat="1" hidden="1">
+    <row r="112" spans="1:9" customFormat="1">
       <c r="A112" s="42"/>
       <c r="B112" s="42" t="s">
         <v>157</v>
@@ -3854,15 +3845,15 @@
       <c r="H112" s="3"/>
       <c r="I112" s="7"/>
     </row>
-    <row r="113" spans="1:9" customFormat="1" hidden="1">
+    <row r="113" spans="1:9" customFormat="1">
       <c r="A113" s="44" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B113" s="44" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C113" s="44" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D113" s="44" t="s">
         <v>9</v>
@@ -3870,12 +3861,12 @@
       <c r="E113" s="17"/>
       <c r="F113" s="44"/>
       <c r="G113" s="12" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="7"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" ht="30" hidden="1">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
         <v>159</v>
@@ -3896,7 +3887,7 @@
       <c r="H114" s="31"/>
       <c r="I114" s="29"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" hidden="1">
       <c r="A115" s="4" t="s">
         <v>174</v>
       </c>
@@ -3912,12 +3903,12 @@
       </c>
       <c r="F115" s="5"/>
       <c r="G115" s="35" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H115" s="31"/>
       <c r="I115" s="29"/>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" hidden="1">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
         <v>176</v>
@@ -3931,12 +3922,12 @@
       </c>
       <c r="F116" s="5"/>
       <c r="G116" s="35" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H116" s="31"/>
       <c r="I116" s="29"/>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" hidden="1">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
         <v>177</v>
@@ -3950,12 +3941,12 @@
       </c>
       <c r="F117" s="5"/>
       <c r="G117" s="35" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H117" s="31"/>
       <c r="I117" s="29"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" hidden="1">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
         <v>178</v>
@@ -3969,12 +3960,12 @@
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="35" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H118" s="31"/>
       <c r="I118" s="29"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" hidden="1">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
         <v>179</v>
@@ -3988,12 +3979,12 @@
       </c>
       <c r="F119" s="5"/>
       <c r="G119" s="35" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H119" s="31"/>
       <c r="I119" s="29"/>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" hidden="1">
       <c r="A120" s="4"/>
       <c r="B120" s="4" t="s">
         <v>180</v>
@@ -4007,12 +3998,12 @@
       </c>
       <c r="F120" s="5"/>
       <c r="G120" s="35" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H120" s="31"/>
       <c r="I120" s="29"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" hidden="1">
       <c r="A121" s="4"/>
       <c r="B121" s="4" t="s">
         <v>181</v>
@@ -4026,12 +4017,12 @@
       </c>
       <c r="F121" s="5"/>
       <c r="G121" s="35" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H121" s="31"/>
       <c r="I121" s="29"/>
     </row>
-    <row r="122" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="122" spans="1:9" ht="15" customHeight="1">
       <c r="A122" s="42" t="s">
         <v>160</v>
       </c>
@@ -4039,7 +4030,7 @@
         <v>161</v>
       </c>
       <c r="C122" s="42" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D122" s="43" t="s">
         <v>9</v>
@@ -4054,13 +4045,13 @@
       <c r="H122" s="31"/>
       <c r="I122" s="29"/>
     </row>
-    <row r="123" spans="1:9" ht="15" hidden="1" customHeight="1">
+    <row r="123" spans="1:9" ht="15" customHeight="1">
       <c r="A123" s="42"/>
       <c r="B123" s="42" t="s">
         <v>162</v>
       </c>
       <c r="C123" s="42" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D123" s="43" t="s">
         <v>9</v>
@@ -4075,7 +4066,7 @@
       <c r="H123" s="31"/>
       <c r="I123" s="29"/>
     </row>
-    <row r="124" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="124" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A124" s="42"/>
       <c r="B124" s="42" t="s">
         <v>163</v>
@@ -4096,7 +4087,7 @@
       <c r="H124" s="3"/>
       <c r="I124" s="7"/>
     </row>
-    <row r="125" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="125" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A125" s="42"/>
       <c r="B125" s="42" t="s">
         <v>164</v>
@@ -4117,13 +4108,13 @@
       <c r="H125" s="3"/>
       <c r="I125" s="7"/>
     </row>
-    <row r="126" spans="1:9" hidden="1">
+    <row r="126" spans="1:9">
       <c r="A126" s="42"/>
       <c r="B126" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C126" s="42" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D126" s="43" t="s">
         <v>9</v>
@@ -4138,7 +4129,7 @@
       <c r="H126" s="31"/>
       <c r="I126" s="29"/>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" hidden="1">
       <c r="A127" s="5"/>
       <c r="B127" s="4" t="s">
         <v>166</v>
@@ -4159,7 +4150,7 @@
       <c r="H127" s="31"/>
       <c r="I127" s="29"/>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" hidden="1">
       <c r="A128" s="4"/>
       <c r="B128" s="4" t="s">
         <v>167</v>
@@ -4175,12 +4166,12 @@
         <v>1</v>
       </c>
       <c r="G128" s="35" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="H128" s="31"/>
       <c r="I128" s="29"/>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" hidden="1">
       <c r="A129" s="4"/>
       <c r="B129" s="4" t="s">
         <v>168</v>
@@ -4196,12 +4187,12 @@
         <v>1</v>
       </c>
       <c r="G129" s="35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H129" s="31"/>
       <c r="I129" s="29"/>
     </row>
-    <row r="130" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="130" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A130" s="42"/>
       <c r="B130" s="42" t="s">
         <v>169</v>
@@ -4222,7 +4213,7 @@
       <c r="H130" s="3"/>
       <c r="I130" s="7"/>
     </row>
-    <row r="131" spans="1:9" ht="15" customHeight="1">
+    <row r="131" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A131" s="4"/>
       <c r="B131" s="4" t="s">
         <v>170</v>
@@ -4243,7 +4234,7 @@
       <c r="H131" s="31"/>
       <c r="I131" s="29"/>
     </row>
-    <row r="132" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="132" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A132" s="1"/>
       <c r="B132" s="12" t="s">
         <v>182</v>
@@ -4262,7 +4253,7 @@
       <c r="H132" s="3"/>
       <c r="I132" s="7"/>
     </row>
-    <row r="133" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="133" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A133" s="42"/>
       <c r="B133" s="42" t="s">
         <v>171</v>
@@ -4304,7 +4295,7 @@
       <c r="H134" s="31"/>
       <c r="I134" s="29"/>
     </row>
-    <row r="135" spans="1:9" ht="15" customHeight="1">
+    <row r="135" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A135" s="4"/>
       <c r="B135" s="4" t="s">
         <v>183</v>
@@ -4320,12 +4311,12 @@
         <v>3</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H135" s="31"/>
       <c r="I135" s="29"/>
     </row>
-    <row r="136" spans="1:9" ht="15" customHeight="1">
+    <row r="136" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A136" s="4"/>
       <c r="B136" s="4" t="s">
         <v>184</v>
@@ -4346,13 +4337,13 @@
       <c r="H136" s="31"/>
       <c r="I136" s="29"/>
     </row>
-    <row r="137" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
+    <row r="137" spans="1:9" customFormat="1" ht="15" customHeight="1">
       <c r="A137" s="42"/>
       <c r="B137" s="42" t="s">
         <v>185</v>
       </c>
       <c r="C137" s="42" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D137" s="43" t="s">
         <v>9</v>
@@ -4367,7 +4358,7 @@
       <c r="H137" s="3"/>
       <c r="I137" s="7"/>
     </row>
-    <row r="138" spans="1:9" customFormat="1" ht="15" customHeight="1">
+    <row r="138" spans="1:9" customFormat="1" ht="15" hidden="1" customHeight="1">
       <c r="A138" s="1"/>
       <c r="B138" s="2" t="s">
         <v>186</v>
@@ -4375,7 +4366,7 @@
       <c r="C138" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D138" s="47" t="s">
+      <c r="D138" s="45" t="s">
         <v>27</v>
       </c>
       <c r="E138" s="20" t="s">
@@ -4385,12 +4376,12 @@
         <v>2</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="7"/>
     </row>
-    <row r="139" spans="1:9" ht="15" customHeight="1">
+    <row r="139" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A139" s="4"/>
       <c r="B139" s="4" t="s">
         <v>187</v>
@@ -4411,7 +4402,7 @@
       <c r="H139" s="31"/>
       <c r="I139" s="29"/>
     </row>
-    <row r="140" spans="1:9" ht="15" customHeight="1">
+    <row r="140" spans="1:9" ht="15" hidden="1" customHeight="1">
       <c r="A140" s="4"/>
       <c r="B140" s="4" t="s">
         <v>188</v>
@@ -4479,7 +4470,7 @@
   <autoFilter ref="A1:F142" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
-        <filter val="N/A"/>
+        <filter val="Completed"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>